<commit_message>
Reduce DuckDB/SQLite extension boilerplate; replace personal test data
DuckDB ext (853→525 lines): unify InitData/InitDataFmt, replace 17 init
trampolines and 20 JSON scalar wrappers with extra_info dispatch,
table-driven registration loop.

SQLite ext (851→438 lines): DEFINE_VTAB macro generates all vtab
boilerplate except Column, replace 25 scalar wrappers with two generic
functions via sqlite3_user_data, table-driven registration.

Replace personal glavel_receipt.pdf with generated test_data/sample.pdf
and regenerate sample.xlsx and sample.docx with fictional data.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/test_data/sample.xlsx
+++ b/test_data/sample.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sales" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,65 +427,265 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Date</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Q4</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Widget A</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
+      <c r="C2" t="n">
+        <v>120</v>
+      </c>
+      <c r="D2" t="n">
+        <v>135</v>
+      </c>
+      <c r="E2" t="n">
+        <v>148</v>
+      </c>
+      <c r="F2" t="n">
+        <v>162</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Widget B</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>200</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2024-02-20</t>
-        </is>
+      <c r="C3" t="n">
+        <v>85</v>
+      </c>
+      <c r="D3" t="n">
+        <v>92</v>
+      </c>
+      <c r="E3" t="n">
+        <v>88</v>
+      </c>
+      <c r="F3" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Widget C</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>300</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2024-03-25</t>
-        </is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Widget A</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>200</v>
+      </c>
+      <c r="D4" t="n">
+        <v>210</v>
+      </c>
+      <c r="E4" t="n">
+        <v>195</v>
+      </c>
+      <c r="F4" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Widget B</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>150</v>
+      </c>
+      <c r="D5" t="n">
+        <v>165</v>
+      </c>
+      <c r="E5" t="n">
+        <v>172</v>
+      </c>
+      <c r="F5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>East</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Gadget C</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>80</v>
+      </c>
+      <c r="E6" t="n">
+        <v>82</v>
+      </c>
+      <c r="F6" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>West</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Gadget C</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>60</v>
+      </c>
+      <c r="D7" t="n">
+        <v>65</v>
+      </c>
+      <c r="E7" t="n">
+        <v>70</v>
+      </c>
+      <c r="F7" t="n">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Total Q1</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>SUM(Sales!C2:C7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Total Q2</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>SUM(Sales!D2:D7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total Q3</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>SUM(Sales!E2:E7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Total Q4</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>SUM(Sales!F2:F7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Grand Total</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>